<commit_message>
test retired population and added new functions
</commit_message>
<xml_diff>
--- a/ageServiceTables/age-service-distribution.xlsx
+++ b/ageServiceTables/age-service-distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyteng/Documents/Brown2021Fall/TPL/pawg/ageServiceTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4B5C0D-1100-A047-9828-7FA0D3A4EECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB8F6C1-9C53-074E-AABF-7D53AAB3D138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="540" windowWidth="28040" windowHeight="16440" xr2:uid="{D26EF8C0-BC42-294E-9500-8C51CEBD4674}"/>
+    <workbookView xWindow="760" yWindow="480" windowWidth="28040" windowHeight="16440" xr2:uid="{D26EF8C0-BC42-294E-9500-8C51CEBD4674}"/>
   </bookViews>
   <sheets>
     <sheet name="Cal-T" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <f>SUM(B2:L2)</f>
+        <f t="shared" ref="M2:M12" si="0">SUM(B2:L2)</f>
         <v>5896</v>
       </c>
     </row>
@@ -589,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <f>SUM(B3:L3)</f>
+        <f t="shared" si="0"/>
         <v>30018</v>
       </c>
     </row>
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <f>SUM(B4:L4)</f>
+        <f t="shared" si="0"/>
         <v>35756</v>
       </c>
     </row>
@@ -673,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <f>SUM(B5:L5)</f>
+        <f t="shared" si="0"/>
         <v>44732</v>
       </c>
     </row>
@@ -715,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <f>SUM(B6:L6)</f>
+        <f t="shared" si="0"/>
         <v>50430</v>
       </c>
     </row>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <f>SUM(B7:L7)</f>
+        <f t="shared" si="0"/>
         <v>50571</v>
       </c>
     </row>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <f>SUM(B8:L8)</f>
+        <f t="shared" si="0"/>
         <v>41432</v>
       </c>
     </row>
@@ -841,7 +841,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <f>SUM(B9:L9)</f>
+        <f t="shared" si="0"/>
         <v>35445</v>
       </c>
     </row>
@@ -883,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="M10">
-        <f>SUM(B10:L10)</f>
+        <f t="shared" si="0"/>
         <v>20702</v>
       </c>
     </row>
@@ -925,7 +925,7 @@
         <v>15</v>
       </c>
       <c r="M11">
-        <f>SUM(B11:L11)</f>
+        <f t="shared" si="0"/>
         <v>7307</v>
       </c>
     </row>
@@ -967,7 +967,7 @@
         <v>84</v>
       </c>
       <c r="M12">
-        <f>SUM(B12:L12)</f>
+        <f t="shared" si="0"/>
         <v>2879</v>
       </c>
     </row>
@@ -980,47 +980,47 @@
         <v>28536</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:M13" si="0">SUM(C2:C12)</f>
+        <f t="shared" ref="C13:M13" si="1">SUM(C2:C12)</f>
         <v>68079</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54204</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54188</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53220</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39492</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17476</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8121</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1534</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>218</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>325168</v>
       </c>
     </row>

</xml_diff>